<commit_message>
Add methods to get bacterium taxonomy by it ID #23
</commit_message>
<xml_diff>
--- a/greg_S_aureus.xlsx
+++ b/greg_S_aureus.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A361AFDA-E8EC-4DC0-A954-32D2DAE84925}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0180C6B-17EC-48D3-AB90-ED4F53D9EC71}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20268" yWindow="816" windowWidth="20376" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="71">
   <si>
     <t>P68</t>
   </si>
@@ -67,21 +67,9 @@
     <t>Sa53Yok</t>
   </si>
   <si>
-    <t>CL&amp;2M</t>
-  </si>
-  <si>
     <t>Sa72Yok</t>
   </si>
   <si>
-    <t>2M</t>
-  </si>
-  <si>
-    <t>SCL&amp;2M</t>
-  </si>
-  <si>
-    <t>OL&amp;2M</t>
-  </si>
-  <si>
     <t>Sa80Yok</t>
   </si>
   <si>
@@ -242,6 +230,9 @@
   </si>
   <si>
     <t>bac/phage</t>
+  </si>
+  <si>
+    <t>NONE</t>
   </si>
 </sst>
 </file>
@@ -629,7 +620,7 @@
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,7 +630,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -801,7 +792,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -819,25 +810,25 @@
     </row>
     <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>6</v>
@@ -845,7 +836,7 @@
     </row>
     <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
@@ -871,7 +862,7 @@
     </row>
     <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>6</v>
@@ -880,16 +871,16 @@
         <v>6</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>7</v>
@@ -897,7 +888,7 @@
     </row>
     <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -915,7 +906,7 @@
     </row>
     <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -935,7 +926,7 @@
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -953,7 +944,7 @@
     </row>
     <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -973,7 +964,7 @@
     </row>
     <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>12</v>
@@ -999,7 +990,7 @@
     </row>
     <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1017,7 +1008,7 @@
     </row>
     <row r="18" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1035,7 +1026,7 @@
     </row>
     <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1053,7 +1044,7 @@
     </row>
     <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1071,7 +1062,7 @@
     </row>
     <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1087,7 +1078,7 @@
     </row>
     <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>12</v>
@@ -1113,7 +1104,7 @@
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1127,7 +1118,7 @@
     </row>
     <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1145,7 +1136,7 @@
     </row>
     <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>12</v>
@@ -1171,7 +1162,7 @@
     </row>
     <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>12</v>
@@ -1193,14 +1184,14 @@
     </row>
     <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>6</v>
@@ -1215,7 +1206,7 @@
     </row>
     <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>7</v>
@@ -1241,14 +1232,14 @@
     </row>
     <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>6</v>
@@ -1257,7 +1248,7 @@
         <v>12</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>7</v>
@@ -1265,7 +1256,7 @@
     </row>
     <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1283,7 +1274,7 @@
     </row>
     <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1293,15 +1284,15 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1323,7 +1314,7 @@
     </row>
     <row r="33" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>6</v>
@@ -1339,7 +1330,7 @@
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>7</v>
@@ -1347,7 +1338,7 @@
     </row>
     <row r="34" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>6</v>
@@ -1371,7 +1362,7 @@
     </row>
     <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1389,7 +1380,7 @@
     </row>
     <row r="36" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>7</v>
@@ -1413,7 +1404,7 @@
     </row>
     <row r="37" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>6</v>
@@ -1437,7 +1428,7 @@
     </row>
     <row r="38" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>6</v>
@@ -1463,7 +1454,7 @@
     </row>
     <row r="39" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>7</v>
@@ -1487,7 +1478,7 @@
     </row>
     <row r="40" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>7</v>
@@ -1499,7 +1490,7 @@
         <v>6</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="2" t="s">
@@ -1509,7 +1500,7 @@
     </row>
     <row r="41" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>7</v>
@@ -1535,7 +1526,7 @@
     </row>
     <row r="42" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>7</v>
@@ -1561,7 +1552,7 @@
     </row>
     <row r="43" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1583,7 +1574,7 @@
     </row>
     <row r="44" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>7</v>
@@ -1607,7 +1598,7 @@
     </row>
     <row r="45" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1629,7 +1620,7 @@
     </row>
     <row r="46" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1651,7 +1642,7 @@
     </row>
     <row r="47" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1669,7 +1660,7 @@
     </row>
     <row r="48" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1687,7 +1678,7 @@
     </row>
     <row r="49" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1705,7 +1696,7 @@
     </row>
     <row r="50" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1723,7 +1714,7 @@
     </row>
     <row r="51" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -1741,7 +1732,7 @@
     </row>
     <row r="52" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1763,7 +1754,7 @@
     </row>
     <row r="53" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1781,7 +1772,7 @@
     </row>
     <row r="54" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>12</v>
@@ -1803,7 +1794,7 @@
     </row>
     <row r="55" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>7</v>
@@ -1812,16 +1803,16 @@
         <v>7</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>6</v>
@@ -1829,7 +1820,7 @@
     </row>
     <row r="56" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>6</v>
@@ -1853,7 +1844,7 @@
     </row>
     <row r="57" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -1875,7 +1866,7 @@
     </row>
     <row r="58" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>7</v>
@@ -1899,7 +1890,7 @@
     </row>
     <row r="59" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -1921,7 +1912,7 @@
     </row>
     <row r="60" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -1939,13 +1930,13 @@
     </row>
     <row r="61" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>6</v>
@@ -1963,7 +1954,7 @@
     </row>
     <row r="62" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>7</v>
@@ -1975,7 +1966,7 @@
         <v>6</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="2" t="s">

</xml_diff>

<commit_message>
Add code to check the interaction type #23
</commit_message>
<xml_diff>
--- a/greg_S_aureus.xlsx
+++ b/greg_S_aureus.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0180C6B-17EC-48D3-AB90-ED4F53D9EC71}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227BDB84-A8A1-4237-AB89-C04243EFFE70}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20268" yWindow="816" windowWidth="20376" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -321,9 +321,6 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="1" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -335,6 +332,9 @@
     </xf>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="1" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -619,13 +619,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -655,7 +656,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -681,15 +682,21 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>-1</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="7">
+        <v>-1</v>
+      </c>
       <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
@@ -701,19 +708,33 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="B4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>-1</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -728,14 +749,18 @@
       <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="7">
+        <v>-1</v>
+      </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="7">
+        <v>-1</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -761,7 +786,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -776,7 +801,9 @@
       <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="7">
+        <v>-1</v>
+      </c>
       <c r="G7" s="2" t="s">
         <v>6</v>
       </c>
@@ -785,7 +812,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -800,7 +827,9 @@
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="7">
+        <v>-1</v>
+      </c>
       <c r="G8" s="2" t="s">
         <v>6</v>
       </c>
@@ -809,7 +838,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -835,7 +864,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -861,7 +890,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -887,16 +916,24 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C12" s="7">
+        <v>-1</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="E12" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F12" s="7">
+        <v>-1</v>
+      </c>
       <c r="G12" s="2" t="s">
         <v>6</v>
       </c>
@@ -905,18 +942,24 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C13" s="7">
+        <v>-1</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="F13" s="7">
+        <v>-1</v>
+      </c>
       <c r="G13" s="2" t="s">
         <v>6</v>
       </c>
@@ -925,16 +968,24 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C14" s="7">
+        <v>-1</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F14" s="7">
+        <v>-1</v>
+      </c>
       <c r="G14" s="2" t="s">
         <v>7</v>
       </c>
@@ -943,18 +994,24 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="B15" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C15" s="7">
+        <v>-1</v>
+      </c>
       <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="7">
+        <v>-1</v>
+      </c>
       <c r="G15" s="2" t="s">
         <v>6</v>
       </c>
@@ -963,7 +1020,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -989,16 +1046,24 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="B17" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C17" s="7">
+        <v>-1</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="E17" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F17" s="7">
+        <v>-1</v>
+      </c>
       <c r="G17" s="2" t="s">
         <v>6</v>
       </c>
@@ -1007,16 +1072,24 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="B18" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C18" s="7">
+        <v>-1</v>
+      </c>
       <c r="D18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="E18" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F18" s="7">
+        <v>-1</v>
+      </c>
       <c r="G18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1025,16 +1098,24 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="B19" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C19" s="7">
+        <v>-1</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>-1</v>
+      </c>
       <c r="G19" s="2" t="s">
         <v>6</v>
       </c>
@@ -1043,16 +1124,24 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="B20" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C20" s="7">
+        <v>-1</v>
+      </c>
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F20" s="7">
+        <v>-1</v>
+      </c>
       <c r="G20" s="2" t="s">
         <v>6</v>
       </c>
@@ -1061,23 +1150,33 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="B21" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C21" s="7">
+        <v>-1</v>
+      </c>
       <c r="D21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="E21" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F21" s="7">
+        <v>-1</v>
+      </c>
       <c r="G21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H21" s="3"/>
+      <c r="H21" s="7">
+        <v>-1</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1103,30 +1202,50 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="B23" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C23" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D23" s="7">
+        <v>-1</v>
+      </c>
+      <c r="E23" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F23" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G23" s="7">
+        <v>-1</v>
+      </c>
       <c r="H23" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="B24" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C24" s="7">
+        <v>-1</v>
+      </c>
       <c r="D24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F24" s="7">
+        <v>-1</v>
+      </c>
       <c r="G24" s="2" t="s">
         <v>12</v>
       </c>
@@ -1135,7 +1254,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1161,20 +1280,24 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="7">
+        <v>-1</v>
+      </c>
       <c r="D26" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="3"/>
+      <c r="F26" s="7">
+        <v>-1</v>
+      </c>
       <c r="G26" s="2" t="s">
         <v>7</v>
       </c>
@@ -1183,20 +1306,24 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="7">
+        <v>-1</v>
+      </c>
       <c r="D27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="3"/>
+      <c r="F27" s="7">
+        <v>-1</v>
+      </c>
       <c r="G27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1205,7 +1332,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1231,13 +1358,15 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="3"/>
+      <c r="C29" s="7">
+        <v>-1</v>
+      </c>
       <c r="D29" s="2" t="s">
         <v>6</v>
       </c>
@@ -1255,16 +1384,24 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
+      <c r="B30" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C30" s="7">
+        <v>-1</v>
+      </c>
       <c r="D30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="E30" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F30" s="7">
+        <v>-1</v>
+      </c>
       <c r="G30" s="2" t="s">
         <v>6</v>
       </c>
@@ -1273,16 +1410,24 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+      <c r="B31" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C31" s="7">
+        <v>-1</v>
+      </c>
       <c r="D31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="E31" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F31" s="7">
+        <v>-1</v>
+      </c>
       <c r="G31" s="2" t="s">
         <v>6</v>
       </c>
@@ -1291,11 +1436,15 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+      <c r="B32" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C32" s="7">
+        <v>-1</v>
+      </c>
       <c r="D32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1313,7 +1462,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1328,7 +1477,9 @@
       <c r="E33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="3"/>
+      <c r="F33" s="7">
+        <v>-1</v>
+      </c>
       <c r="G33" s="2" t="s">
         <v>6</v>
       </c>
@@ -1337,7 +1488,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1352,7 +1503,9 @@
       <c r="E34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="3"/>
+      <c r="F34" s="7">
+        <v>-1</v>
+      </c>
       <c r="G34" s="2" t="s">
         <v>6</v>
       </c>
@@ -1361,16 +1514,24 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+      <c r="B35" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C35" s="7">
+        <v>-1</v>
+      </c>
       <c r="D35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="E35" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F35" s="7">
+        <v>-1</v>
+      </c>
       <c r="G35" s="2" t="s">
         <v>6</v>
       </c>
@@ -1379,7 +1540,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -1394,7 +1555,9 @@
       <c r="E36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="3"/>
+      <c r="F36" s="7">
+        <v>-1</v>
+      </c>
       <c r="G36" s="2" t="s">
         <v>6</v>
       </c>
@@ -1403,7 +1566,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1418,7 +1581,9 @@
       <c r="E37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F37" s="3"/>
+      <c r="F37" s="7">
+        <v>-1</v>
+      </c>
       <c r="G37" s="2" t="s">
         <v>6</v>
       </c>
@@ -1427,7 +1592,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1453,7 +1618,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1468,7 +1633,9 @@
       <c r="E39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="3"/>
+      <c r="F39" s="7">
+        <v>-1</v>
+      </c>
       <c r="G39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1477,7 +1644,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1492,14 +1659,18 @@
       <c r="E40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F40" s="3"/>
+      <c r="F40" s="7">
+        <v>-1</v>
+      </c>
       <c r="G40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H40" s="3"/>
+      <c r="H40" s="7">
+        <v>-1</v>
+      </c>
     </row>
     <row r="41" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1525,7 +1696,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1551,11 +1722,15 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
+      <c r="B43" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C43" s="7">
+        <v>-1</v>
+      </c>
       <c r="D43" s="2" t="s">
         <v>6</v>
       </c>
@@ -1573,7 +1748,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -1588,7 +1763,9 @@
       <c r="E44" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="3"/>
+      <c r="F44" s="7">
+        <v>-1</v>
+      </c>
       <c r="G44" s="2" t="s">
         <v>7</v>
       </c>
@@ -1597,11 +1774,15 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+      <c r="B45" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C45" s="7">
+        <v>-1</v>
+      </c>
       <c r="D45" s="2" t="s">
         <v>6</v>
       </c>
@@ -1619,11 +1800,15 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
+      <c r="B46" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C46" s="7">
+        <v>-1</v>
+      </c>
       <c r="D46" s="2" t="s">
         <v>7</v>
       </c>
@@ -1641,16 +1826,24 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
+      <c r="B47" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C47" s="7">
+        <v>-1</v>
+      </c>
       <c r="D47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
+      <c r="E47" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F47" s="7">
+        <v>-1</v>
+      </c>
       <c r="G47" s="2" t="s">
         <v>6</v>
       </c>
@@ -1659,16 +1852,24 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
+      <c r="B48" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C48" s="7">
+        <v>-1</v>
+      </c>
       <c r="D48" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
+      <c r="E48" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F48" s="7">
+        <v>-1</v>
+      </c>
       <c r="G48" s="2" t="s">
         <v>6</v>
       </c>
@@ -1677,16 +1878,24 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
+      <c r="B49" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C49" s="7">
+        <v>-1</v>
+      </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
+      <c r="E49" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F49" s="7">
+        <v>-1</v>
+      </c>
       <c r="G49" s="2" t="s">
         <v>6</v>
       </c>
@@ -1695,16 +1904,24 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
+      <c r="B50" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C50" s="7">
+        <v>-1</v>
+      </c>
       <c r="D50" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
+      <c r="E50" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F50" s="7">
+        <v>-1</v>
+      </c>
       <c r="G50" s="2" t="s">
         <v>6</v>
       </c>
@@ -1713,16 +1930,24 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
+      <c r="B51" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C51" s="7">
+        <v>-1</v>
+      </c>
       <c r="D51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
+      <c r="E51" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F51" s="7">
+        <v>-1</v>
+      </c>
       <c r="G51" s="2" t="s">
         <v>6</v>
       </c>
@@ -1731,11 +1956,15 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
+      <c r="B52" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C52" s="7">
+        <v>-1</v>
+      </c>
       <c r="D52" s="2" t="s">
         <v>6</v>
       </c>
@@ -1753,16 +1982,24 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
+      <c r="B53" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C53" s="7">
+        <v>-1</v>
+      </c>
       <c r="D53" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
+      <c r="E53" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F53" s="7">
+        <v>-1</v>
+      </c>
       <c r="G53" s="2" t="s">
         <v>6</v>
       </c>
@@ -1771,20 +2008,24 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C54" s="3"/>
+      <c r="C54" s="7">
+        <v>-1</v>
+      </c>
       <c r="D54" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F54" s="3"/>
+      <c r="F54" s="7">
+        <v>-1</v>
+      </c>
       <c r="G54" s="2" t="s">
         <v>6</v>
       </c>
@@ -1793,7 +2034,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="6" t="s">
         <v>61</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -1819,7 +2060,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="6" t="s">
         <v>62</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -1834,7 +2075,9 @@
       <c r="E56" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F56" s="3"/>
+      <c r="F56" s="7">
+        <v>-1</v>
+      </c>
       <c r="G56" s="2" t="s">
         <v>6</v>
       </c>
@@ -1843,11 +2086,15 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
+      <c r="B57" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C57" s="7">
+        <v>-1</v>
+      </c>
       <c r="D57" s="2" t="s">
         <v>6</v>
       </c>
@@ -1865,7 +2112,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -1880,7 +2127,9 @@
       <c r="E58" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F58" s="3"/>
+      <c r="F58" s="7">
+        <v>-1</v>
+      </c>
       <c r="G58" s="2" t="s">
         <v>6</v>
       </c>
@@ -1889,11 +2138,15 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
+      <c r="B59" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C59" s="7">
+        <v>-1</v>
+      </c>
       <c r="D59" s="2" t="s">
         <v>6</v>
       </c>
@@ -1911,16 +2164,24 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
+      <c r="B60" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C60" s="7">
+        <v>-1</v>
+      </c>
       <c r="D60" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
+      <c r="E60" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F60" s="7">
+        <v>-1</v>
+      </c>
       <c r="G60" s="2" t="s">
         <v>6</v>
       </c>
@@ -1929,7 +2190,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B61" s="2" t="s">
@@ -1944,7 +2205,9 @@
       <c r="E61" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F61" s="3"/>
+      <c r="F61" s="7">
+        <v>-1</v>
+      </c>
       <c r="G61" s="2" t="s">
         <v>6</v>
       </c>
@@ -1953,7 +2216,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -1968,7 +2231,9 @@
       <c r="E62" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F62" s="3"/>
+      <c r="F62" s="7">
+        <v>-1</v>
+      </c>
       <c r="G62" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Update script that insert datagreg into db #23
</commit_message>
<xml_diff>
--- a/greg_S_aureus.xlsx
+++ b/greg_S_aureus.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227BDB84-A8A1-4237-AB89-C04243EFFE70}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B82A150-F1A7-4401-B40A-D9AEF2756E79}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20268" yWindow="816" windowWidth="20376" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="72">
   <si>
     <t>P68</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>NONE</t>
+  </si>
+  <si>
+    <t>-1</t>
   </si>
 </sst>
 </file>
@@ -619,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,8 +697,8 @@
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="7">
-        <v>-1</v>
+      <c r="E3" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>7</v>
@@ -2243,5 +2246,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>